<commit_message>
answers and maxdiff for 2j
</commit_message>
<xml_diff>
--- a/Maxdiff-llama-answers/llama_responses_sofia.xlsx
+++ b/Maxdiff-llama-answers/llama_responses_sofia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sofia/Desktop/cognitive-project/Maxdiff-llama-answers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843EF4FC-37D1-544A-813C-106F4625A291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8EECF8-9A52-FB4B-9F00-5FE4E56EA992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="780" windowWidth="27500" windowHeight="16940" xr2:uid="{17896173-B686-5A49-A532-34CA6A521573}"/>
+    <workbookView xWindow="3660" yWindow="500" windowWidth="27500" windowHeight="16940" activeTab="1" xr2:uid="{17896173-B686-5A49-A532-34CA6A521573}"/>
   </bookViews>
   <sheets>
     <sheet name="2i" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="3d" sheetId="4" r:id="rId4"/>
     <sheet name="3e" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2j'!$A$1:$F$106</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2262" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2472" uniqueCount="209">
   <si>
     <t>tree:blood</t>
   </si>
@@ -1020,7 +1023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA74B965-D331-3241-9CBD-F5E9AFB1C773}">
   <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -3021,11 +3024,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7450A181-60A6-2846-B36D-457463E5FC00}">
   <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="E104" sqref="E104:F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -3060,6 +3068,12 @@
       <c r="D2" t="s">
         <v>48</v>
       </c>
+      <c r="E2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -3074,6 +3088,12 @@
       <c r="D3" t="s">
         <v>75</v>
       </c>
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -3088,6 +3108,12 @@
       <c r="D4" t="s">
         <v>54</v>
       </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -3102,6 +3128,12 @@
       <c r="D5" t="s">
         <v>79</v>
       </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -3116,6 +3148,12 @@
       <c r="D6" t="s">
         <v>58</v>
       </c>
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -3130,6 +3168,12 @@
       <c r="D7" t="s">
         <v>67</v>
       </c>
+      <c r="E7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -3144,6 +3188,12 @@
       <c r="D8" t="s">
         <v>74</v>
       </c>
+      <c r="E8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -3158,6 +3208,12 @@
       <c r="D9" t="s">
         <v>65</v>
       </c>
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -3172,6 +3228,12 @@
       <c r="D10" t="s">
         <v>63</v>
       </c>
+      <c r="E10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -3186,6 +3248,12 @@
       <c r="D11" t="s">
         <v>55</v>
       </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -3200,6 +3268,12 @@
       <c r="D12" t="s">
         <v>66</v>
       </c>
+      <c r="E12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -3214,6 +3288,12 @@
       <c r="D13" t="s">
         <v>51</v>
       </c>
+      <c r="E13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -3228,6 +3308,12 @@
       <c r="D14" t="s">
         <v>83</v>
       </c>
+      <c r="E14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -3242,6 +3328,12 @@
       <c r="D15" t="s">
         <v>84</v>
       </c>
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -3256,8 +3348,14 @@
       <c r="D16" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -3270,8 +3368,14 @@
       <c r="D17" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -3284,8 +3388,14 @@
       <c r="D18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -3298,8 +3408,14 @@
       <c r="D19" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -3312,8 +3428,14 @@
       <c r="D20" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -3326,8 +3448,14 @@
       <c r="D21" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -3340,8 +3468,14 @@
       <c r="D22" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -3354,8 +3488,14 @@
       <c r="D23" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -3368,8 +3508,14 @@
       <c r="D24" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -3382,8 +3528,14 @@
       <c r="D25" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -3396,8 +3548,14 @@
       <c r="D26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>75</v>
       </c>
@@ -3410,8 +3568,14 @@
       <c r="D27" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -3424,8 +3588,14 @@
       <c r="D28" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -3438,8 +3608,14 @@
       <c r="D29" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>80</v>
       </c>
@@ -3452,8 +3628,14 @@
       <c r="D30" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>85</v>
       </c>
@@ -3466,8 +3648,14 @@
       <c r="D31" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>78</v>
+      </c>
+      <c r="F31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -3480,8 +3668,14 @@
       <c r="D32" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>49</v>
+      </c>
+      <c r="F32" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -3494,8 +3688,14 @@
       <c r="D33" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -3508,8 +3708,14 @@
       <c r="D34" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -3522,8 +3728,14 @@
       <c r="D35" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" t="s">
+        <v>74</v>
+      </c>
+      <c r="F35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>61</v>
       </c>
@@ -3536,8 +3748,14 @@
       <c r="D36" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" t="s">
+        <v>84</v>
+      </c>
+      <c r="F36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>60</v>
       </c>
@@ -3550,8 +3768,14 @@
       <c r="D37" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>82</v>
       </c>
@@ -3564,8 +3788,14 @@
       <c r="D38" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" t="s">
+        <v>83</v>
+      </c>
+      <c r="F38" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>66</v>
       </c>
@@ -3578,8 +3808,14 @@
       <c r="D39" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>63</v>
       </c>
@@ -3592,8 +3828,14 @@
       <c r="D40" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -3606,8 +3848,14 @@
       <c r="D41" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" t="s">
+        <v>76</v>
+      </c>
+      <c r="F41" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>75</v>
       </c>
@@ -3620,8 +3868,14 @@
       <c r="D42" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" t="s">
+        <v>46</v>
+      </c>
+      <c r="F42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -3634,8 +3888,14 @@
       <c r="D43" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" t="s">
+        <v>70</v>
+      </c>
+      <c r="F43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>80</v>
       </c>
@@ -3648,8 +3908,14 @@
       <c r="D44" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" t="s">
+        <v>70</v>
+      </c>
+      <c r="F44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -3662,8 +3928,14 @@
       <c r="D45" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" t="s">
+        <v>84</v>
+      </c>
+      <c r="F45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>83</v>
       </c>
@@ -3676,8 +3948,14 @@
       <c r="D46" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" t="s">
+        <v>50</v>
+      </c>
+      <c r="F46" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>62</v>
       </c>
@@ -3690,8 +3968,14 @@
       <c r="D47" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" t="s">
+        <v>52</v>
+      </c>
+      <c r="F47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>78</v>
       </c>
@@ -3704,8 +3988,14 @@
       <c r="D48" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48" t="s">
+        <v>72</v>
+      </c>
+      <c r="F48" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>85</v>
       </c>
@@ -3718,8 +4008,14 @@
       <c r="D49" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" t="s">
+        <v>82</v>
+      </c>
+      <c r="F49" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -3732,8 +4028,14 @@
       <c r="D50" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50" t="s">
+        <v>63</v>
+      </c>
+      <c r="F50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -3746,8 +4048,14 @@
       <c r="D51" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51" t="s">
+        <v>76</v>
+      </c>
+      <c r="F51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -3760,8 +4068,14 @@
       <c r="D52" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52" t="s">
+        <v>66</v>
+      </c>
+      <c r="F52" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -3774,8 +4088,14 @@
       <c r="D53" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53" t="s">
+        <v>74</v>
+      </c>
+      <c r="F53" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>64</v>
       </c>
@@ -3788,8 +4108,14 @@
       <c r="D54" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54" t="s">
+        <v>55</v>
+      </c>
+      <c r="F54" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>46</v>
       </c>
@@ -3802,8 +4128,14 @@
       <c r="D55" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55" t="s">
+        <v>82</v>
+      </c>
+      <c r="F55" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>74</v>
       </c>
@@ -3816,8 +4148,14 @@
       <c r="D56" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56" t="s">
+        <v>72</v>
+      </c>
+      <c r="F56" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>78</v>
       </c>
@@ -3830,8 +4168,14 @@
       <c r="D57" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57" t="s">
+        <v>76</v>
+      </c>
+      <c r="F57" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>54</v>
       </c>
@@ -3844,8 +4188,14 @@
       <c r="D58" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58" t="s">
+        <v>81</v>
+      </c>
+      <c r="F58" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>49</v>
       </c>
@@ -3858,8 +4208,14 @@
       <c r="D59" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59" t="s">
+        <v>83</v>
+      </c>
+      <c r="F59" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>71</v>
       </c>
@@ -3872,8 +4228,14 @@
       <c r="D60" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60" t="s">
+        <v>58</v>
+      </c>
+      <c r="F60" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>63</v>
       </c>
@@ -3886,8 +4248,14 @@
       <c r="D61" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61" t="s">
+        <v>59</v>
+      </c>
+      <c r="F61" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>73</v>
       </c>
@@ -3900,8 +4268,14 @@
       <c r="D62" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62" t="s">
+        <v>79</v>
+      </c>
+      <c r="F62" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>84</v>
       </c>
@@ -3914,8 +4288,14 @@
       <c r="D63" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63" t="s">
+        <v>55</v>
+      </c>
+      <c r="F63" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>53</v>
       </c>
@@ -3928,8 +4308,14 @@
       <c r="D64" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" t="s">
+        <v>57</v>
+      </c>
+      <c r="F64" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>68</v>
       </c>
@@ -3942,8 +4328,14 @@
       <c r="D65" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65" t="s">
+        <v>73</v>
+      </c>
+      <c r="F65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>55</v>
       </c>
@@ -3956,8 +4348,14 @@
       <c r="D66" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66" t="s">
+        <v>46</v>
+      </c>
+      <c r="F66" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -3970,8 +4368,14 @@
       <c r="D67" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67" t="s">
+        <v>45</v>
+      </c>
+      <c r="F67" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>53</v>
       </c>
@@ -3984,8 +4388,14 @@
       <c r="D68" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68" t="s">
+        <v>74</v>
+      </c>
+      <c r="F68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>61</v>
       </c>
@@ -3998,8 +4408,14 @@
       <c r="D69" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69" t="s">
+        <v>65</v>
+      </c>
+      <c r="F69" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>47</v>
       </c>
@@ -4012,8 +4428,14 @@
       <c r="D70" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70" t="s">
+        <v>50</v>
+      </c>
+      <c r="F70" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>72</v>
       </c>
@@ -4026,8 +4448,14 @@
       <c r="D71" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71" t="s">
+        <v>84</v>
+      </c>
+      <c r="F71" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>56</v>
       </c>
@@ -4040,8 +4468,14 @@
       <c r="D72" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72" t="s">
+        <v>49</v>
+      </c>
+      <c r="F72" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>78</v>
       </c>
@@ -4054,8 +4488,14 @@
       <c r="D73" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73" t="s">
+        <v>59</v>
+      </c>
+      <c r="F73" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>60</v>
       </c>
@@ -4068,8 +4508,14 @@
       <c r="D74" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74" t="s">
+        <v>81</v>
+      </c>
+      <c r="F74" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -4082,8 +4528,14 @@
       <c r="D75" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75" t="s">
+        <v>63</v>
+      </c>
+      <c r="F75" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>83</v>
       </c>
@@ -4096,8 +4548,14 @@
       <c r="D76" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76" t="s">
+        <v>84</v>
+      </c>
+      <c r="F76" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>85</v>
       </c>
@@ -4110,8 +4568,14 @@
       <c r="D77" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77" t="s">
+        <v>82</v>
+      </c>
+      <c r="F77" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>45</v>
       </c>
@@ -4124,8 +4588,14 @@
       <c r="D78" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78" t="s">
+        <v>46</v>
+      </c>
+      <c r="F78" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>49</v>
       </c>
@@ -4138,8 +4608,14 @@
       <c r="D79" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79" t="s">
+        <v>50</v>
+      </c>
+      <c r="F79" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>53</v>
       </c>
@@ -4152,8 +4628,14 @@
       <c r="D80" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80" t="s">
+        <v>55</v>
+      </c>
+      <c r="F80" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>57</v>
       </c>
@@ -4166,8 +4648,14 @@
       <c r="D81" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81" t="s">
+        <v>58</v>
+      </c>
+      <c r="F81" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>61</v>
       </c>
@@ -4180,8 +4668,14 @@
       <c r="D82" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82" t="s">
+        <v>63</v>
+      </c>
+      <c r="F82" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>65</v>
       </c>
@@ -4194,8 +4688,14 @@
       <c r="D83" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83" t="s">
+        <v>66</v>
+      </c>
+      <c r="F83" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>69</v>
       </c>
@@ -4208,8 +4708,14 @@
       <c r="D84" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84" t="s">
+        <v>70</v>
+      </c>
+      <c r="F84" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>73</v>
       </c>
@@ -4222,8 +4728,14 @@
       <c r="D85" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E85" t="s">
+        <v>76</v>
+      </c>
+      <c r="F85" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>52</v>
       </c>
@@ -4236,8 +4748,14 @@
       <c r="D86" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86" t="s">
+        <v>76</v>
+      </c>
+      <c r="F86" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>67</v>
       </c>
@@ -4250,8 +4768,14 @@
       <c r="D87" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87" t="s">
+        <v>71</v>
+      </c>
+      <c r="F87" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>56</v>
       </c>
@@ -4264,8 +4788,14 @@
       <c r="D88" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88" t="s">
+        <v>74</v>
+      </c>
+      <c r="F88" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>59</v>
       </c>
@@ -4278,8 +4808,14 @@
       <c r="D89" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89" t="s">
+        <v>45</v>
+      </c>
+      <c r="F89" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>47</v>
       </c>
@@ -4292,8 +4828,14 @@
       <c r="D90" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E90" t="s">
+        <v>55</v>
+      </c>
+      <c r="F90" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>57</v>
       </c>
@@ -4306,8 +4848,14 @@
       <c r="D91" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E91" t="s">
+        <v>81</v>
+      </c>
+      <c r="F91" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>69</v>
       </c>
@@ -4320,8 +4868,14 @@
       <c r="D92" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E92" t="s">
+        <v>83</v>
+      </c>
+      <c r="F92" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>54</v>
       </c>
@@ -4334,8 +4888,14 @@
       <c r="D93" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E93" t="s">
+        <v>51</v>
+      </c>
+      <c r="F93" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>85</v>
       </c>
@@ -4348,8 +4908,14 @@
       <c r="D94" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E94" t="s">
+        <v>49</v>
+      </c>
+      <c r="F94" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>65</v>
       </c>
@@ -4362,8 +4928,14 @@
       <c r="D95" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E95" t="s">
+        <v>72</v>
+      </c>
+      <c r="F95" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>48</v>
       </c>
@@ -4376,8 +4948,14 @@
       <c r="D96" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E96" t="s">
+        <v>52</v>
+      </c>
+      <c r="F96" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>66</v>
       </c>
@@ -4390,8 +4968,14 @@
       <c r="D97" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E97" t="s">
+        <v>51</v>
+      </c>
+      <c r="F97" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>75</v>
       </c>
@@ -4404,8 +4988,14 @@
       <c r="D98" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E98" t="s">
+        <v>53</v>
+      </c>
+      <c r="F98" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>83</v>
       </c>
@@ -4418,8 +5008,14 @@
       <c r="D99" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E99" t="s">
+        <v>58</v>
+      </c>
+      <c r="F99" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>85</v>
       </c>
@@ -4432,8 +5028,14 @@
       <c r="D100" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E100" t="s">
+        <v>71</v>
+      </c>
+      <c r="F100" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>70</v>
       </c>
@@ -4446,8 +5048,14 @@
       <c r="D101" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E101" t="s">
+        <v>74</v>
+      </c>
+      <c r="F101" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>63</v>
       </c>
@@ -4460,8 +5068,14 @@
       <c r="D102" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E102" t="s">
+        <v>55</v>
+      </c>
+      <c r="F102" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>69</v>
       </c>
@@ -4474,8 +5088,14 @@
       <c r="D103" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E103" t="s">
+        <v>46</v>
+      </c>
+      <c r="F103" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>77</v>
       </c>
@@ -4488,8 +5108,14 @@
       <c r="D104" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E104" t="s">
+        <v>60</v>
+      </c>
+      <c r="F104" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>65</v>
       </c>
@@ -4502,8 +5128,14 @@
       <c r="D105" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E105" t="s">
+        <v>59</v>
+      </c>
+      <c r="F105" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>81</v>
       </c>
@@ -4514,6 +5146,12 @@
         <v>67</v>
       </c>
       <c r="D106" t="s">
+        <v>47</v>
+      </c>
+      <c r="E106" t="s">
+        <v>84</v>
+      </c>
+      <c r="F106" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>